<commit_message>
Fixed multiple instances recorded as unique entries
</commit_message>
<xml_diff>
--- a/SysArch.xlsx
+++ b/SysArch.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="56">
   <si>
     <t>BlockType</t>
   </si>
@@ -67,7 +67,31 @@
     <t>2YpdEY8oORx3fjk5kcs5-2</t>
   </si>
   <si>
+    <t>BSPD2</t>
+  </si>
+  <si>
     <t>qhaE7OJ2hAVIAAOIQZVo-1</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-1</t>
+  </si>
+  <si>
+    <t>BrakeSensor2</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-2</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-3</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-4</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-5</t>
+  </si>
+  <si>
+    <t>MRsK-TLKyB-mq6uifq8Z-6</t>
   </si>
   <si>
     <t>NPC</t>
@@ -507,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,24 +584,24 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -585,16 +609,100 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +720,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -624,18 +732,18 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -644,36 +752,36 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -718,80 +826,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +989,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -890,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -898,13 +1006,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +1030,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -931,7 +1039,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -939,10 +1047,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -955,7 +1063,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -963,7 +1071,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -972,27 +1080,27 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1001,23 +1109,52 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
       <c r="I2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1026,7 +1163,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1034,10 +1171,10 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1046,42 +1183,42 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1090,35 +1227,79 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="M2" t="s">
         <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>